<commit_message>
Added resistors to BOM
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard V2/Parts_List.xlsx
+++ b/Hardware/Boards/Motherboard V2/Parts_List.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Eagle_Parts_List" sheetId="2" r:id="rId2"/>
     <sheet name="Scratch_Pad" sheetId="4" r:id="rId3"/>
+    <sheet name="Complete Parts List" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="220">
   <si>
     <t>Part</t>
   </si>
@@ -661,13 +662,28 @@
   </si>
   <si>
     <t>Capacitors - 1206 Footprint</t>
+  </si>
+  <si>
+    <t>Resistors 1206 Footprint</t>
+  </si>
+  <si>
+    <t>330 Ohm</t>
+  </si>
+  <si>
+    <t>120 Ohm</t>
+  </si>
+  <si>
+    <t>1 Kohm</t>
+  </si>
+  <si>
+    <t>10 Kohm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,6 +715,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -721,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -735,6 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1039,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,50 +1270,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>214</v>
-      </c>
-    </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="6">
-        <v>2</v>
-      </c>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="6">
-        <v>1</v>
-      </c>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="6">
-        <v>29</v>
-      </c>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="6">
-        <v>1</v>
-      </c>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="6">
-        <v>1</v>
-      </c>
+      <c r="B32" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1309,7 +1304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2955,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,7 +2959,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
@@ -3153,7 +3148,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
@@ -3165,7 +3160,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -3177,7 +3172,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>103</v>
       </c>
@@ -3189,7 +3184,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>106</v>
       </c>
@@ -3201,7 +3196,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -3212,1008 +3207,631 @@
         <v>109</v>
       </c>
       <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="3">
-        <v>330</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1206</v>
+        <v>155</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="3">
-        <v>120</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1206</v>
+        <v>158</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B24" s="3">
-        <v>120</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1206</v>
+        <v>159</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="3">
-        <v>120</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1206</v>
+        <v>160</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" s="3">
-        <v>120</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1206</v>
+        <v>161</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="3">
-        <v>120</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1206</v>
+        <v>162</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="3">
-        <v>120</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1206</v>
+        <v>163</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="3">
-        <v>120</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1206</v>
+        <v>164</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="3">
-        <v>120</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1206</v>
+        <v>165</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" s="3">
-        <v>120</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1206</v>
+        <v>166</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B32" s="3">
-        <v>120</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1206</v>
+        <v>167</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" s="3">
-        <v>120</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1206</v>
+        <v>168</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" s="3">
-        <v>120</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1206</v>
+        <v>169</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" s="3">
-        <v>120</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1206</v>
+        <v>170</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" s="3">
-        <v>120</v>
-      </c>
-      <c r="C36" s="3">
-        <v>1206</v>
+        <v>171</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B37" s="3">
-        <v>120</v>
-      </c>
-      <c r="C37" s="3">
-        <v>1206</v>
+        <v>172</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" s="3">
-        <v>120</v>
-      </c>
-      <c r="C38" s="3">
-        <v>1206</v>
+        <v>173</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" s="3">
-        <v>120</v>
-      </c>
-      <c r="C39" s="3">
-        <v>1206</v>
+        <v>174</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="3">
-        <v>120</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1206</v>
+        <v>175</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" s="3">
-        <v>120</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1206</v>
+        <v>178</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="3">
-        <v>120</v>
-      </c>
-      <c r="C42" s="3">
-        <v>1206</v>
+        <v>180</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B43" s="3">
-        <v>120</v>
-      </c>
-      <c r="C43" s="3">
-        <v>1206</v>
+        <v>183</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" s="3">
-        <v>120</v>
-      </c>
-      <c r="C44" s="3">
-        <v>1206</v>
+        <v>185</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" s="3">
-        <v>120</v>
+        <v>188</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="C45" s="3">
-        <v>1206</v>
+        <v>60050685100</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" s="3">
-        <v>120</v>
-      </c>
-      <c r="C46" s="3">
-        <v>1206</v>
+        <v>190</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="3">
-        <v>120</v>
-      </c>
-      <c r="C47" s="3">
-        <v>1206</v>
+        <v>193</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48" s="3">
-        <v>120</v>
-      </c>
-      <c r="C48" s="3">
-        <v>1206</v>
+        <v>194</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B49" s="3">
-        <v>120</v>
-      </c>
-      <c r="C49" s="3">
-        <v>1206</v>
+        <v>195</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B50" s="3">
-        <v>120</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1206</v>
+        <v>196</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B51" s="3">
-        <v>120</v>
-      </c>
-      <c r="C51" s="3">
-        <v>1206</v>
+        <v>197</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B52" s="3">
-        <v>120</v>
-      </c>
-      <c r="C52" s="3">
-        <v>1206</v>
+        <v>198</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B53" s="3">
-        <v>120</v>
-      </c>
-      <c r="C53" s="3">
-        <v>1206</v>
+        <v>200</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B54" s="3">
-        <v>120</v>
-      </c>
-      <c r="C54" s="3">
-        <v>1206</v>
+        <v>203</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B55" s="3">
-        <v>120</v>
-      </c>
-      <c r="C55" s="3">
-        <v>1206</v>
+        <v>206</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B56" s="3">
-        <v>120</v>
-      </c>
-      <c r="C56" s="3">
-        <v>1206</v>
+        <v>207</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B57" s="3">
-        <v>120</v>
-      </c>
-      <c r="C57" s="3">
-        <v>1206</v>
+        <v>208</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B58" s="3">
-        <v>120</v>
-      </c>
-      <c r="C58" s="3">
-        <v>1206</v>
+        <v>209</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C59" s="3">
-        <v>1206</v>
+        <v>201</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C60" s="3">
-        <v>1206</v>
+        <v>212</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" s="3">
-        <v>1206</v>
-      </c>
+      <c r="B61" s="3"/>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="3">
-        <v>1206</v>
-      </c>
       <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C63" s="3">
-        <v>1206</v>
-      </c>
       <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>157</v>
-      </c>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>177</v>
-      </c>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>36</v>
-      </c>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>182</v>
-      </c>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>184</v>
-      </c>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>187</v>
-      </c>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C87" s="3">
-        <v>60050685100</v>
-      </c>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>192</v>
-      </c>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>192</v>
-      </c>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>192</v>
-      </c>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>192</v>
-      </c>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>192</v>
-      </c>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>192</v>
-      </c>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>199</v>
-      </c>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>202</v>
-      </c>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>205</v>
-      </c>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>202</v>
-      </c>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>202</v>
-      </c>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>202</v>
-      </c>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>202</v>
-      </c>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>202</v>
-      </c>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>213</v>
-      </c>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="3"/>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
@@ -4287,6 +3905,119 @@
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated need to buy list.
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard V2/Parts_List.xlsx
+++ b/Hardware/Boards/Motherboard V2/Parts_List.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Complete Parts List" sheetId="5" r:id="rId2"/>
+    <sheet name="Complete Parts List" sheetId="5" r:id="rId1"/>
+    <sheet name="Need_To_Buy" sheetId="6" r:id="rId2"/>
     <sheet name="Eagle_Raw_Parts_List" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="254">
   <si>
     <t>Part</t>
   </si>
@@ -33,9 +33,6 @@
     <t>https://www.sparkfun.com/products/9473</t>
   </si>
   <si>
-    <t>Dual 4:1 Muxes</t>
-  </si>
-  <si>
     <t>http://www.newark.com/nxp/74hc4052d-653/ic-analog-mux-dmux-dual-4-x-1/dp/78R7402</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>http://www.adafruit.com/products/746</t>
   </si>
   <si>
-    <t>Digital Temp</t>
-  </si>
-  <si>
     <t>http://www.mouser.com/ProductDetail/Maxim-Integrated/MAX3077EESA+/?qs=sGAEpiMZZMuobhpKLk3hh6ov3TfCBqZhbNybjDy0atQ%3d</t>
   </si>
   <si>
@@ -60,27 +54,9 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>5mm 2 pin Screw Terminals</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8432</t>
-  </si>
-  <si>
-    <t>Green LED</t>
-  </si>
-  <si>
-    <t>Red LED</t>
-  </si>
-  <si>
     <t>LCD</t>
   </si>
   <si>
-    <t>Trimpot</t>
-  </si>
-  <si>
-    <t>http://www.adafruit.com/products/393#Description</t>
-  </si>
-  <si>
     <t>RJ-45 Jacks</t>
   </si>
   <si>
@@ -739,6 +715,69 @@
   </si>
   <si>
     <t>3.3v Regulator</t>
+  </si>
+  <si>
+    <t>Quantity for One Motherboard</t>
+  </si>
+  <si>
+    <t>40+</t>
+  </si>
+  <si>
+    <t>22pF Capacitors</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12061a220jat2a/capacitor-ceramic-22pf-100v-c0g/dp/96K4783</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/SPBT2632C2AAT2/?qs=sGAEpiMZZMsGelYiB%252bjhZr92XQgUe9SaTh31rlV%252bAv4%3d</t>
+  </si>
+  <si>
+    <t>100nF Capacitors</t>
+  </si>
+  <si>
+    <t>1uF Capacitors</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12063c105kat2a/capacitor-ceramic-1uf-25v-x7r/dp/96K4787</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12061c104jat2a/capacitor-ceramic-0-1uf-100v-x7r/dp/96M1466</t>
+  </si>
+  <si>
+    <t>red LED</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/lumex/sml-lx1206ic-tr/led-red-3-2mm-x-1-6mm-6mcd-635nm/dp/80K7325</t>
+  </si>
+  <si>
+    <t>green LED</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/lumex/sml-lx1206gw-tr/led-green-3-2mm-x-1-6mm-10mcd/dp/77K7035</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>u.FL Connectors</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Taoglas/RECE-20279-001E-01/?qs=sGAEpiMZZMvRX1W9I</t>
+  </si>
+  <si>
+    <t>Male 0.1 inch headers</t>
+  </si>
+  <si>
+    <t>Female 0.1 inch header</t>
+  </si>
+  <si>
+    <t>At least 40</t>
+  </si>
+  <si>
+    <t>at least 46</t>
   </si>
 </sst>
 </file>
@@ -786,7 +825,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,6 +835,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,21 +858,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1130,190 +1177,498 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D9" r:id="rId3" location="Description"/>
-    <hyperlink ref="D11" r:id="rId4"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="A43" sqref="A43:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="126.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="126.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="5">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26">
+        <v>36</v>
+      </c>
+      <c r="C26" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40" s="9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>217</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>218</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>219</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D11" r:id="rId4"/>
+    <hyperlink ref="D33" r:id="rId5" display="http://www.newark.com/stmicroelectronics/ld1117s33ctr/ic-ldo-volt-reg-3-3v-0-8a-sot/dp/89K0626?CMP=AFC-OP"/>
+    <hyperlink ref="D18" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1321,357 +1676,161 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>233</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>220</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
+      <c r="C5" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>217</v>
-      </c>
-      <c r="B7">
+      <c r="A6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6">
         <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>226</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>222</v>
+      <c r="A13" t="s">
+        <v>218</v>
       </c>
       <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>224</v>
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="6">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B25">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>211</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>212</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>229</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>233</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>234</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>236</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>238</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>239</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>225</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>226</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>227</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>230</v>
-      </c>
-      <c r="B44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>232</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>235</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>22</v>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C32" r:id="rId4"/>
-    <hyperlink ref="C36" r:id="rId5"/>
-    <hyperlink ref="C11" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5" display="http://www.newark.com/stmicroelectronics/ld1117s33ctr/ic-ldo-volt-reg-3-3v-0-8a-sot/dp/89K0626?CMP=AFC-OP"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C10" r:id="rId7"/>
+    <hyperlink ref="C14" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1692,59 +1851,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>26</v>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3">
         <v>1206</v>
@@ -1754,10 +1913,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3">
         <v>1206</v>
@@ -1766,10 +1925,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3">
         <v>1206</v>
@@ -1778,10 +1937,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3">
         <v>1206</v>
@@ -1790,10 +1949,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3">
         <v>1206</v>
@@ -1802,10 +1961,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3">
         <v>1206</v>
@@ -1814,10 +1973,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3">
         <v>1206</v>
@@ -1826,10 +1985,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3">
         <v>1206</v>
@@ -1838,10 +1997,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3">
         <v>1206</v>
@@ -1850,10 +2009,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3">
         <v>1206</v>
@@ -1862,10 +2021,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>1206</v>
@@ -1874,10 +2033,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3">
         <v>1206</v>
@@ -1886,10 +2045,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3">
         <v>1206</v>
@@ -1898,10 +2057,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3">
         <v>1206</v>
@@ -1910,10 +2069,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3">
         <v>1206</v>
@@ -1922,10 +2081,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3">
         <v>1206</v>
@@ -1934,10 +2093,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3">
         <v>1206</v>
@@ -1946,10 +2105,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3">
         <v>1206</v>
@@ -1958,10 +2117,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3">
         <v>1206</v>
@@ -1970,10 +2129,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
         <v>1206</v>
@@ -1982,10 +2141,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3">
         <v>1206</v>
@@ -1994,10 +2153,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3">
         <v>1206</v>
@@ -2006,10 +2165,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3">
         <v>1206</v>
@@ -2018,10 +2177,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3">
         <v>1206</v>
@@ -2030,10 +2189,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3">
         <v>1206</v>
@@ -2042,10 +2201,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3">
         <v>1206</v>
@@ -2054,10 +2213,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C31" s="3">
         <v>1206</v>
@@ -2066,10 +2225,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C32" s="3">
         <v>1206</v>
@@ -2078,10 +2237,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3">
         <v>1206</v>
@@ -2090,10 +2249,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3">
         <v>1206</v>
@@ -2102,10 +2261,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C35" s="3">
         <v>1206</v>
@@ -2114,10 +2273,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C36" s="3">
         <v>1206</v>
@@ -2126,10 +2285,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C37" s="3">
         <v>1206</v>
@@ -2138,10 +2297,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C38" s="3">
         <v>1206</v>
@@ -2150,178 +2309,178 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C53" s="3">
         <v>402</v>
@@ -2330,19 +2489,19 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B55" s="3">
         <v>330</v>
@@ -2354,7 +2513,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B56" s="3">
         <v>120</v>
@@ -2366,7 +2525,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B57" s="3">
         <v>120</v>
@@ -2378,7 +2537,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B58" s="3">
         <v>120</v>
@@ -2390,7 +2549,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B59" s="3">
         <v>120</v>
@@ -2402,7 +2561,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B60" s="3">
         <v>120</v>
@@ -2414,7 +2573,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B61" s="3">
         <v>120</v>
@@ -2426,7 +2585,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B62" s="3">
         <v>120</v>
@@ -2438,7 +2597,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B63" s="3">
         <v>120</v>
@@ -2450,7 +2609,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B64" s="3">
         <v>120</v>
@@ -2462,7 +2621,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B65" s="3">
         <v>120</v>
@@ -2474,7 +2633,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B66" s="3">
         <v>120</v>
@@ -2486,7 +2645,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B67" s="3">
         <v>120</v>
@@ -2498,7 +2657,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B68" s="3">
         <v>120</v>
@@ -2510,7 +2669,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B69" s="3">
         <v>120</v>
@@ -2522,7 +2681,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B70" s="3">
         <v>120</v>
@@ -2534,7 +2693,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B71" s="3">
         <v>120</v>
@@ -2546,7 +2705,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B72" s="3">
         <v>120</v>
@@ -2558,7 +2717,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B73" s="3">
         <v>120</v>
@@ -2570,7 +2729,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B74" s="3">
         <v>120</v>
@@ -2582,7 +2741,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B75" s="3">
         <v>120</v>
@@ -2594,7 +2753,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B76" s="3">
         <v>120</v>
@@ -2606,7 +2765,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B77" s="3">
         <v>120</v>
@@ -2618,7 +2777,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B78" s="3">
         <v>120</v>
@@ -2630,7 +2789,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B79" s="3">
         <v>120</v>
@@ -2642,7 +2801,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B80" s="3">
         <v>120</v>
@@ -2654,7 +2813,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B81" s="3">
         <v>120</v>
@@ -2666,7 +2825,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B82" s="3">
         <v>120</v>
@@ -2678,7 +2837,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B83" s="3">
         <v>120</v>
@@ -2690,7 +2849,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B84" s="3">
         <v>120</v>
@@ -2702,7 +2861,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B85" s="3">
         <v>120</v>
@@ -2714,7 +2873,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B86" s="3">
         <v>120</v>
@@ -2726,7 +2885,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B87" s="3">
         <v>120</v>
@@ -2738,7 +2897,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B88" s="3">
         <v>120</v>
@@ -2750,7 +2909,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B89" s="3">
         <v>120</v>
@@ -2762,7 +2921,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B90" s="3">
         <v>120</v>
@@ -2774,7 +2933,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B91" s="3">
         <v>120</v>
@@ -2786,10 +2945,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C92" s="3">
         <v>1206</v>
@@ -2798,10 +2957,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C93" s="3">
         <v>1206</v>
@@ -2810,10 +2969,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C94" s="3">
         <v>1206</v>
@@ -2822,10 +2981,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C95" s="3">
         <v>1206</v>
@@ -2834,10 +2993,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C96" s="3">
         <v>1206</v>
@@ -2846,286 +3005,286 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D98" s="3"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D99" s="3"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D100" s="3"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D101" s="3"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D102" s="3"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D110" s="3"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D116" s="3"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D117" s="3"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C120" s="3">
         <v>60050685100</v>
@@ -3134,181 +3293,181 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D121" s="3"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D122" s="3"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D124" s="3"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D128" s="3"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D129" s="3"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D130" s="3"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D131" s="3"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D132" s="3"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D135" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updated Motherboard V2 with new LEDs
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard V2/Parts_List.xlsx
+++ b/Hardware/Boards/Motherboard V2/Parts_List.xlsx
@@ -750,15 +750,9 @@
     <t>red LED</t>
   </si>
   <si>
-    <t>http://www.newark.com/lumex/sml-lx1206ic-tr/led-red-3-2mm-x-1-6mm-6mcd-635nm/dp/80K7325</t>
-  </si>
-  <si>
     <t>green LED</t>
   </si>
   <si>
-    <t>http://www.newark.com/lumex/sml-lx1206gw-tr/led-green-3-2mm-x-1-6mm-10mcd/dp/77K7035</t>
-  </si>
-  <si>
     <t>u.FL Connectors</t>
   </si>
   <si>
@@ -775,6 +769,12 @@
   </si>
   <si>
     <t>at least 46</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/LH-N974-KN-1/?qs=sGAEpiMZZMt82OzCyDsLFAV097Vn80XJzM0DIFS2How%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/LG-N971-KN-1/?qs=sGAEpiMZZMseGfSY3csMkRFGmqWc9Zh4pe067IXnwes%3d</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1177,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,18 +1272,18 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1299,29 +1299,29 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -1331,9 +1331,8 @@
     <hyperlink ref="C6" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5" display="http://www.newark.com/stmicroelectronics/ld1117s33ctr/ic-ldo-volt-reg-3-3v-0-8a-sot/dp/89K0626?CMP=AFC-OP"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C10" r:id="rId7"/>
-    <hyperlink ref="C13" r:id="rId8"/>
+    <hyperlink ref="C13" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting Aduino Proxy TCP Software
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard V2/Parts_List.xlsx
+++ b/Hardware/Boards/Motherboard V2/Parts_List.xlsx
@@ -822,7 +822,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,6 +841,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -855,7 +861,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -872,6 +878,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1177,7 +1184,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A15" sqref="A15:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1206,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>213</v>
       </c>
       <c r="B2">
@@ -1221,7 +1228,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="10" t="s">
         <v>235</v>
       </c>
       <c r="B4">
@@ -1232,7 +1239,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>238</v>
       </c>
       <c r="B5">
@@ -1243,7 +1250,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>239</v>
       </c>
       <c r="B6">
@@ -1254,7 +1261,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
         <v>226</v>
       </c>
       <c r="B8">
@@ -1298,7 +1305,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>245</v>
       </c>
       <c r="B13">
@@ -1309,7 +1316,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="10" t="s">
         <v>247</v>
       </c>
       <c r="B15" t="s">
@@ -1317,7 +1324,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>248</v>
       </c>
       <c r="B16" t="s">
@@ -1342,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:B43"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1714,7 @@
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B37">
@@ -1823,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added temp connector to BOM
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard V2/Parts_List.xlsx
+++ b/Hardware/Boards/Motherboard V2/Parts_List.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="18460" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Need_To_Buy" sheetId="6" r:id="rId1"/>
     <sheet name="Complete Parts List" sheetId="5" r:id="rId2"/>
     <sheet name="Eagle_Raw_Parts_List" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="256">
   <si>
     <t>Part</t>
   </si>
@@ -775,6 +780,15 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/LG-N971-KN-1/?qs=sGAEpiMZZMseGfSY3csMkRFGmqWc9Zh4pe067IXnwes%3d</t>
+  </si>
+  <si>
+    <t>Temp Sensor Male connector</t>
+  </si>
+  <si>
+    <t>1 required</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-11-2036/?qs=sGAEpiMZZMs%252bGHln7q6pmyYFY3tENhoZIUoV5tIp%2fcs%3d</t>
   </si>
 </sst>
 </file>
@@ -1181,20 +1195,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A16"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1205,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
         <v>213</v>
       </c>
@@ -1216,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -1227,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="10" t="s">
         <v>235</v>
       </c>
@@ -1238,7 +1252,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="7" t="s">
         <v>238</v>
       </c>
@@ -1249,7 +1263,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="7" t="s">
         <v>239</v>
       </c>
@@ -1260,7 +1274,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="10" t="s">
         <v>226</v>
       </c>
@@ -1271,7 +1285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>243</v>
       </c>
@@ -1282,7 +1296,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -1293,7 +1307,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1304,7 +1318,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
         <v>245</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="10" t="s">
         <v>247</v>
       </c>
@@ -1323,12 +1337,23 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="10" t="s">
         <v>248</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1342,6 +1367,11 @@
     <hyperlink ref="C9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1353,15 +1383,15 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="126.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="126.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18">
       <c r="A2" s="6" t="s">
         <v>210</v>
       </c>
@@ -1383,7 +1413,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -1397,7 +1427,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -1411,12 +1441,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -1427,7 +1457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1441,7 +1471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>206</v>
       </c>
@@ -1455,7 +1485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -1469,7 +1499,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>232</v>
       </c>
@@ -1483,16 +1513,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="6" t="s">
         <v>214</v>
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -1506,7 +1536,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1520,14 +1550,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
         <v>200</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1541,7 +1571,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1552,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1563,7 +1593,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1574,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1585,12 +1615,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="6" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
         <v>202</v>
       </c>
@@ -1601,7 +1631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -1612,7 +1642,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>204</v>
       </c>
@@ -1623,7 +1653,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>205</v>
       </c>
@@ -1634,12 +1664,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -1650,7 +1680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>225</v>
       </c>
@@ -1661,7 +1691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>226</v>
       </c>
@@ -1675,7 +1705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>228</v>
       </c>
@@ -1689,7 +1719,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>230</v>
       </c>
@@ -1701,7 +1731,7 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>231</v>
       </c>
@@ -1713,7 +1743,7 @@
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="7" t="s">
         <v>15</v>
       </c>
@@ -1727,12 +1757,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="6" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -1743,7 +1773,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>217</v>
       </c>
@@ -1754,7 +1784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>218</v>
       </c>
@@ -1765,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>219</v>
       </c>
@@ -1776,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>222</v>
       </c>
@@ -1787,7 +1817,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>224</v>
       </c>
@@ -1795,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>227</v>
       </c>
@@ -1803,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1852,12 @@
     <hyperlink ref="D10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1834,15 +1869,15 @@
       <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1865,7 +1900,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1877,7 +1912,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1890,7 +1925,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1903,7 +1938,7 @@
       <c r="D5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1915,7 +1950,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1927,7 +1962,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1939,7 +1974,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -1951,7 +1986,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -1963,7 +1998,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -1975,7 +2010,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1987,7 +2022,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1999,7 +2034,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -2011,7 +2046,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -2023,7 +2058,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -2035,7 +2070,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
@@ -2047,7 +2082,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2094,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>43</v>
       </c>
@@ -2071,7 +2106,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -2083,7 +2118,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -2095,7 +2130,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -2107,7 +2142,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
@@ -2119,7 +2154,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
@@ -2131,7 +2166,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -2143,7 +2178,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -2155,7 +2190,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2167,7 +2202,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
@@ -2179,7 +2214,7 @@
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -2191,7 +2226,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -2203,7 +2238,7 @@
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
@@ -2215,7 +2250,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
@@ -2227,7 +2262,7 @@
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>59</v>
       </c>
@@ -2239,7 +2274,7 @@
       </c>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>60</v>
       </c>
@@ -2251,7 +2286,7 @@
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
         <v>61</v>
       </c>
@@ -2263,7 +2298,7 @@
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>63</v>
       </c>
@@ -2275,7 +2310,7 @@
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
         <v>64</v>
       </c>
@@ -2287,7 +2322,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
         <v>65</v>
       </c>
@@ -2299,7 +2334,7 @@
       </c>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
         <v>66</v>
       </c>
@@ -2311,7 +2346,7 @@
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>69</v>
       </c>
@@ -2323,7 +2358,7 @@
       </c>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
         <v>71</v>
       </c>
@@ -2335,7 +2370,7 @@
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
         <v>74</v>
       </c>
@@ -2347,7 +2382,7 @@
       </c>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
         <v>76</v>
       </c>
@@ -2359,7 +2394,7 @@
       </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
         <v>77</v>
       </c>
@@ -2371,7 +2406,7 @@
       </c>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>78</v>
       </c>
@@ -2383,7 +2418,7 @@
       </c>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2395,7 +2430,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
         <v>81</v>
       </c>
@@ -2407,7 +2442,7 @@
       </c>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
         <v>84</v>
       </c>
@@ -2419,7 +2454,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
         <v>85</v>
       </c>
@@ -2431,7 +2466,7 @@
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
         <v>86</v>
       </c>
@@ -2443,7 +2478,7 @@
       </c>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
         <v>87</v>
       </c>
@@ -2455,7 +2490,7 @@
       </c>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
         <v>89</v>
       </c>
@@ -2467,7 +2502,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
         <v>92</v>
       </c>
@@ -2479,7 +2514,7 @@
       </c>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
         <v>12</v>
       </c>
@@ -2491,7 +2526,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
         <v>96</v>
       </c>
@@ -2503,7 +2538,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
         <v>97</v>
       </c>
@@ -2515,7 +2550,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
         <v>98</v>
       </c>
@@ -2527,7 +2562,7 @@
       </c>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
         <v>99</v>
       </c>
@@ -2539,7 +2574,7 @@
       </c>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
         <v>100</v>
       </c>
@@ -2551,7 +2586,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
         <v>101</v>
       </c>
@@ -2563,7 +2598,7 @@
       </c>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="3" t="s">
         <v>102</v>
       </c>
@@ -2575,7 +2610,7 @@
       </c>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
         <v>103</v>
       </c>
@@ -2587,7 +2622,7 @@
       </c>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="3" t="s">
         <v>104</v>
       </c>
@@ -2599,7 +2634,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
         <v>105</v>
       </c>
@@ -2611,7 +2646,7 @@
       </c>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="3" t="s">
         <v>106</v>
       </c>
@@ -2623,7 +2658,7 @@
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
         <v>107</v>
       </c>
@@ -2635,7 +2670,7 @@
       </c>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="3" t="s">
         <v>108</v>
       </c>
@@ -2647,7 +2682,7 @@
       </c>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="3" t="s">
         <v>109</v>
       </c>
@@ -2659,7 +2694,7 @@
       </c>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
         <v>110</v>
       </c>
@@ -2671,7 +2706,7 @@
       </c>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
         <v>111</v>
       </c>
@@ -2683,7 +2718,7 @@
       </c>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
         <v>112</v>
       </c>
@@ -2695,7 +2730,7 @@
       </c>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="3" t="s">
         <v>113</v>
       </c>
@@ -2707,7 +2742,7 @@
       </c>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
         <v>114</v>
       </c>
@@ -2719,7 +2754,7 @@
       </c>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
         <v>115</v>
       </c>
@@ -2731,7 +2766,7 @@
       </c>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
         <v>116</v>
       </c>
@@ -2743,7 +2778,7 @@
       </c>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
         <v>117</v>
       </c>
@@ -2755,7 +2790,7 @@
       </c>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
         <v>118</v>
       </c>
@@ -2767,7 +2802,7 @@
       </c>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="3" t="s">
         <v>119</v>
       </c>
@@ -2779,7 +2814,7 @@
       </c>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="3" t="s">
         <v>120</v>
       </c>
@@ -2791,7 +2826,7 @@
       </c>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
         <v>121</v>
       </c>
@@ -2803,7 +2838,7 @@
       </c>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
         <v>122</v>
       </c>
@@ -2815,7 +2850,7 @@
       </c>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
         <v>123</v>
       </c>
@@ -2827,7 +2862,7 @@
       </c>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
         <v>124</v>
       </c>
@@ -2839,7 +2874,7 @@
       </c>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
         <v>125</v>
       </c>
@@ -2851,7 +2886,7 @@
       </c>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="3" t="s">
         <v>126</v>
       </c>
@@ -2863,7 +2898,7 @@
       </c>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="3" t="s">
         <v>127</v>
       </c>
@@ -2875,7 +2910,7 @@
       </c>
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
         <v>128</v>
       </c>
@@ -2887,7 +2922,7 @@
       </c>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
         <v>129</v>
       </c>
@@ -2899,7 +2934,7 @@
       </c>
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
         <v>130</v>
       </c>
@@ -2911,7 +2946,7 @@
       </c>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
         <v>131</v>
       </c>
@@ -2923,7 +2958,7 @@
       </c>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
         <v>132</v>
       </c>
@@ -2935,7 +2970,7 @@
       </c>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="3" t="s">
         <v>133</v>
       </c>
@@ -2947,7 +2982,7 @@
       </c>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="3" t="s">
         <v>135</v>
       </c>
@@ -2959,7 +2994,7 @@
       </c>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="3" t="s">
         <v>137</v>
       </c>
@@ -2971,7 +3006,7 @@
       </c>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="3" t="s">
         <v>139</v>
       </c>
@@ -2983,7 +3018,7 @@
       </c>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="3" t="s">
         <v>140</v>
       </c>
@@ -2995,7 +3030,7 @@
       </c>
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="3" t="s">
         <v>141</v>
       </c>
@@ -3007,7 +3042,7 @@
       </c>
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="3" t="s">
         <v>144</v>
       </c>
@@ -3019,7 +3054,7 @@
       </c>
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="3" t="s">
         <v>145</v>
       </c>
@@ -3031,7 +3066,7 @@
       </c>
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="3" t="s">
         <v>146</v>
       </c>
@@ -3043,7 +3078,7 @@
       </c>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="3" t="s">
         <v>147</v>
       </c>
@@ -3055,7 +3090,7 @@
       </c>
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
         <v>148</v>
       </c>
@@ -3067,7 +3102,7 @@
       </c>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="3" t="s">
         <v>149</v>
       </c>
@@ -3079,7 +3114,7 @@
       </c>
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="3" t="s">
         <v>150</v>
       </c>
@@ -3091,7 +3126,7 @@
       </c>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="3" t="s">
         <v>151</v>
       </c>
@@ -3103,7 +3138,7 @@
       </c>
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
         <v>152</v>
       </c>
@@ -3115,7 +3150,7 @@
       </c>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
         <v>153</v>
       </c>
@@ -3127,7 +3162,7 @@
       </c>
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="3" t="s">
         <v>154</v>
       </c>
@@ -3139,7 +3174,7 @@
       </c>
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
         <v>155</v>
       </c>
@@ -3151,7 +3186,7 @@
       </c>
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
         <v>156</v>
       </c>
@@ -3163,7 +3198,7 @@
       </c>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
         <v>157</v>
       </c>
@@ -3175,7 +3210,7 @@
       </c>
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
         <v>158</v>
       </c>
@@ -3187,7 +3222,7 @@
       </c>
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
         <v>159</v>
       </c>
@@ -3199,7 +3234,7 @@
       </c>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="3" t="s">
         <v>160</v>
       </c>
@@ -3211,7 +3246,7 @@
       </c>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="3" t="s">
         <v>161</v>
       </c>
@@ -3223,7 +3258,7 @@
       </c>
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="3" t="s">
         <v>164</v>
       </c>
@@ -3235,7 +3270,7 @@
       </c>
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="3" t="s">
         <v>166</v>
       </c>
@@ -3247,7 +3282,7 @@
       </c>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="3" t="s">
         <v>169</v>
       </c>
@@ -3259,7 +3294,7 @@
       </c>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="3" t="s">
         <v>171</v>
       </c>
@@ -3271,7 +3306,7 @@
       </c>
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="3" t="s">
         <v>174</v>
       </c>
@@ -3283,7 +3318,7 @@
       </c>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="3" t="s">
         <v>176</v>
       </c>
@@ -3295,7 +3330,7 @@
       </c>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="3" t="s">
         <v>179</v>
       </c>
@@ -3307,7 +3342,7 @@
       </c>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="3" t="s">
         <v>180</v>
       </c>
@@ -3319,7 +3354,7 @@
       </c>
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="3" t="s">
         <v>181</v>
       </c>
@@ -3331,7 +3366,7 @@
       </c>
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="3" t="s">
         <v>182</v>
       </c>
@@ -3343,7 +3378,7 @@
       </c>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="3" t="s">
         <v>183</v>
       </c>
@@ -3355,7 +3390,7 @@
       </c>
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="3" t="s">
         <v>184</v>
       </c>
@@ -3367,7 +3402,7 @@
       </c>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="3" t="s">
         <v>186</v>
       </c>
@@ -3379,7 +3414,7 @@
       </c>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="3" t="s">
         <v>189</v>
       </c>
@@ -3391,7 +3426,7 @@
       </c>
       <c r="D129" s="3"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="3" t="s">
         <v>192</v>
       </c>
@@ -3403,7 +3438,7 @@
       </c>
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="3" t="s">
         <v>193</v>
       </c>
@@ -3415,7 +3450,7 @@
       </c>
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="3" t="s">
         <v>194</v>
       </c>
@@ -3427,7 +3462,7 @@
       </c>
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="3" t="s">
         <v>195</v>
       </c>
@@ -3439,7 +3474,7 @@
       </c>
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="3" t="s">
         <v>196</v>
       </c>
@@ -3451,7 +3486,7 @@
       </c>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="3" t="s">
         <v>197</v>
       </c>
@@ -3463,11 +3498,16 @@
       </c>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="B136" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new parts lists for backup parts
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Motherboard V2/Parts_List.xlsx
+++ b/Hardware/Boards/Motherboard V2/Parts_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="18465" windowHeight="10680"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="18465" windowHeight="10680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Need_To_Buy" sheetId="6" r:id="rId1"/>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>

</xml_diff>